<commit_message>
New added config files
</commit_message>
<xml_diff>
--- a/rrd/AppData/Lead_ConfigData.xlsx
+++ b/rrd/AppData/Lead_ConfigData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rai Sigh\git\RRD_Opportunity\rrd\AppData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15D604C-CDC5-4A0F-B9C2-83F38953DF32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F03D0A-65E7-4F7C-A2F0-9F01478CE1CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lead_Config1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="Lead_Config13" sheetId="25" r:id="rId13"/>
     <sheet name="Lead_Config14" sheetId="26" r:id="rId14"/>
     <sheet name="Lead_Config15" sheetId="27" r:id="rId15"/>
+    <sheet name="Lead_Config16" sheetId="28" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="27">
   <si>
     <t>None</t>
   </si>
@@ -865,7 +866,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{773BBFE3-4E1A-4EEF-B4C7-55FCF7B0D769}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -929,6 +932,76 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDD857B-F2AA-432E-89EB-4CEC4552AF65}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7C0B44-C7BA-474A-AAA2-62A627FC138C}">
   <dimension ref="A1:D2"/>
@@ -1076,7 +1149,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4986849C-3E33-4FBB-9A89-1A9D2169038E}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
New Lead Configuration => 16/09/2020
</commit_message>
<xml_diff>
--- a/rrd/AppData/Lead_ConfigData.xlsx
+++ b/rrd/AppData/Lead_ConfigData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rai Sigh\git\RRD_Opportunity\rrd\AppData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FBC9A4-F554-4115-ADCC-3532BCC041C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49A19F1-5C44-4510-85F1-2616E27881B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="15" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="27" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lead_Config1" sheetId="1" r:id="rId1"/>
@@ -24,15 +24,27 @@
     <sheet name="Lead_Config9" sheetId="21" r:id="rId9"/>
     <sheet name="Lead_Config10" sheetId="22" r:id="rId10"/>
     <sheet name="Lead_Config11" sheetId="23" r:id="rId11"/>
-    <sheet name="Lead_Config12" sheetId="24" r:id="rId12"/>
-    <sheet name="Lead_Config13" sheetId="25" r:id="rId13"/>
-    <sheet name="Lead_Config14" sheetId="26" r:id="rId14"/>
-    <sheet name="Lead_Config15" sheetId="27" r:id="rId15"/>
-    <sheet name="Lead_Config16" sheetId="28" r:id="rId16"/>
-    <sheet name="Lead_Config17" sheetId="29" r:id="rId17"/>
-    <sheet name="Lead_Config18" sheetId="30" r:id="rId18"/>
-    <sheet name="Lead_Config19" sheetId="31" r:id="rId19"/>
-    <sheet name="Lead_Config20" sheetId="32" r:id="rId20"/>
+    <sheet name="Sheet1" sheetId="34" r:id="rId12"/>
+    <sheet name="Lead_Config12" sheetId="24" r:id="rId13"/>
+    <sheet name="Lead_Config13" sheetId="25" r:id="rId14"/>
+    <sheet name="Lead_Config14" sheetId="26" r:id="rId15"/>
+    <sheet name="Lead_Config15" sheetId="27" r:id="rId16"/>
+    <sheet name="Lead_Config16" sheetId="28" r:id="rId17"/>
+    <sheet name="Lead_Config17" sheetId="29" r:id="rId18"/>
+    <sheet name="Lead_Config18" sheetId="30" r:id="rId19"/>
+    <sheet name="Lead_Config19" sheetId="31" r:id="rId20"/>
+    <sheet name="Lead_Config20" sheetId="32" r:id="rId21"/>
+    <sheet name="Lead_Config21" sheetId="33" r:id="rId22"/>
+    <sheet name="Lead_Config22" sheetId="35" r:id="rId23"/>
+    <sheet name="Lead_Config23" sheetId="36" r:id="rId24"/>
+    <sheet name="Lead_Config24" sheetId="37" r:id="rId25"/>
+    <sheet name="Lead_Config25" sheetId="38" r:id="rId26"/>
+    <sheet name="Lead_Config26" sheetId="39" r:id="rId27"/>
+    <sheet name="Lead_Config27" sheetId="40" r:id="rId28"/>
+    <sheet name="Lead_Config28" sheetId="41" r:id="rId29"/>
+    <sheet name="Lead_Config29" sheetId="42" r:id="rId30"/>
+    <sheet name="Lead_Config30" sheetId="43" r:id="rId31"/>
+    <sheet name="Lead_Config31" sheetId="44" r:id="rId32"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -44,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="27">
   <si>
     <t>None</t>
   </si>
@@ -595,7 +607,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8643E788-546D-4CD2-BBCC-69B921BA96DF}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -660,6 +674,18 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FB3029-3DAD-47D6-8B56-37CBCD999E50}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B58113ED-4625-47DA-90CD-42BA4B18AC40}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -727,7 +753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221885D0-B23F-44B0-98C8-66B172F06777}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -797,7 +823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0023955A-D2D5-4198-98BD-8D406906B18F}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -866,7 +892,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{773BBFE3-4E1A-4EEF-B4C7-55FCF7B0D769}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -934,7 +960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDD857B-F2AA-432E-89EB-4CEC4552AF65}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1002,7 +1028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6406EE3-176B-437A-87F0-AD1D3746711D}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1070,7 +1096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B056EF-6DC7-4564-8998-EBC4190C2242}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1138,7 +1164,54 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7C0B44-C7BA-474A-AAA2-62A627FC138C}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA87271-D4D2-4D93-8D02-9F573D8F8F12}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1206,60 +1279,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7C0B44-C7BA-474A-AAA2-62A627FC138C}">
-  <dimension ref="A1:D2"/>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37404401-9603-48E2-9678-10DE3E3D1B0B}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37404401-9603-48E2-9678-10DE3E3D1B0B}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1323,6 +1347,558 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32AD71C-3831-41B6-954E-3B1D3E86C812}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E932D9-CB7C-4806-B08A-705182331ABB}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346E5697-6DB3-4177-A2F4-701437ACC3FE}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6401ACAA-C921-40CF-BD41-3A38CD231B0E}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F358E65-3E29-4F24-A5FD-9285A82F345A}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1F0DC0-9F33-4814-8E7C-E2CB26726F40}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B45C8B-A1E7-44B0-8754-0CF92E1C287F}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAA323E-1122-4E1D-8B59-CD3ABF6E224A}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20989C05-60DF-4C67-8A75-A703FDE9C969}">
   <dimension ref="A1:D2"/>
@@ -1370,6 +1946,209 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C9969A-3DDB-472E-9AD2-E5C7733486BF}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64535BC6-B29F-425C-9D83-4353E095F20A}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B5E00C-D398-4399-A8B0-0773FAC5E4BB}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C2D50E0-6BF1-49CD-9074-0FF03E24C19E}">
   <dimension ref="A1:D2"/>

</xml_diff>

<commit_message>
Commit request = 23/09
</commit_message>
<xml_diff>
--- a/rrd/AppData/Lead_ConfigData.xlsx
+++ b/rrd/AppData/Lead_ConfigData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rai Sigh\git\RRD_Opportunity\rrd\AppData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26769443-BEEB-4B21-895D-4CC7101094BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DBE08E1-15CD-468A-A7FF-DC80F3004E78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="15" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="16" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lead_Config1" sheetId="1" r:id="rId1"/>
@@ -964,7 +964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDD857B-F2AA-432E-89EB-4CEC4552AF65}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1285,7 +1285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37404401-9603-48E2-9678-10DE3E3D1B0B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Commit request => 01/10/2020
</commit_message>
<xml_diff>
--- a/rrd/AppData/Lead_ConfigData.xlsx
+++ b/rrd/AppData/Lead_ConfigData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rai Sigh\git\RRD_Opportunity\rrd\AppData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DBE08E1-15CD-468A-A7FF-DC80F3004E78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AA08FB-5826-4750-8CF1-6C505D8D2B43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="16" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="26" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lead_Config1" sheetId="1" r:id="rId1"/>
@@ -1285,7 +1285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37404401-9603-48E2-9678-10DE3E3D1B0B}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1699,8 +1699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1F0DC0-9F33-4814-8E7C-E2CB26726F40}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2020,7 +2020,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64535BC6-B29F-425C-9D83-4353E095F20A}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>